<commit_message>
Update Estrategias de pruebas
</commit_message>
<xml_diff>
--- a/Documentos/PTP_Juan_Cajoia_Jonathan_ Garcia_26092023 .xlsx
+++ b/Documentos/PTP_Juan_Cajoia_Jonathan_ Garcia_26092023 .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C7013A8-135D-425A-A1E6-2BE14D381865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{36F89E65-23F6-4CFF-8FAF-8912E2678A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D20512B1-8783-41FD-B729-50DEFE0AFE11}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Estrategia de Pruebas" sheetId="1" r:id="rId1"/>
     <sheet name="Bugs" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="232">
+  <si>
+    <t>Team 15</t>
+  </si>
+  <si>
+    <t>Integrantes:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Juan Esteban Cajiao Madero y Jonathan Andres Garcia Rodriguez  </t>
+  </si>
+  <si>
+    <t>Enlace Pagina Web:</t>
+  </si>
+  <si>
+    <t>https://www.booking.com/</t>
+  </si>
   <si>
     <t>ID</t>
   </si>
@@ -72,42 +87,130 @@
     <t xml:space="preserve">ATOMATIZABLE </t>
   </si>
   <si>
-    <t>Team 15</t>
-  </si>
-  <si>
-    <t>Integrantes:</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Juan Esteban Cajiao Madero y Jonathan Andres Garcia Rodriguez  </t>
-  </si>
-  <si>
-    <t>Enlace Pagina Web:</t>
-  </si>
-  <si>
-    <t>https://www.booking.com/</t>
+    <t>Register Successful</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario se podrá registrar en la  plataforma Booking </t>
+  </si>
+  <si>
+    <t>Usuario: jagarcia8578@soy.sena.edu.co
+Contraseña: Prueba123456</t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina web https://www.booking.com/ 
+2. El usuario debe ubicar el cursor en la parte superior derecha haciendo clic en la opción "Hazte una Cuenta" 
+3. El usuario ingresara el correo electrónico en el campo "Indica tu dirección de E-mail"
+4. El usuario debe hacer clic en el botón denominado "Continuar con E-mail"
+5. El usuario debe ingresar la contraseña en el campo "Introduce tu contraseña"
+6. El usuario debe confirmar la contraseña en el campo "Confirma tu contraseña"
+7.  El usuario debe hacer clic en el botón denominado "Crear una cuentan"
+8. El usuario podrá visualizar la interfaz donde le permite configurar la cuenta.</t>
+  </si>
+  <si>
+    <t>Registro exitoso</t>
+  </si>
+  <si>
+    <t>Jonathan García y Juan Cajiao</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>Register Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario no se podrá registrar en la  plataforma Booking </t>
+  </si>
+  <si>
+    <t>Usuario: jagarcia8578@soy</t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina web https://www.booking.com/ 
+2. El usuario debe ubicar el cursor en la parte superior derecha haciendo clic en la opción "Hazte una Cuenta" 
+3. El usuario ingresara el correo electrónico en el campo "Indica tu dirección de E-mail"
+4. El usuario debe hacer clic en el botón denominado "Continuar con E-mail"
+5. El usuario evidenciara el siguiente aviso "Comprueba si el e-mail que has introducido es correcto"</t>
+  </si>
+  <si>
+    <t>Registro fallido</t>
+  </si>
+  <si>
+    <t>Failed registration empty fields in email</t>
+  </si>
+  <si>
+    <t>El usuario no se podrá registrar en la  plataforma Booking por campo vacio Email</t>
+  </si>
+  <si>
+    <t>ususario: "Campos vacios"</t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina web https://www.booking.com/ 
+2. El usuario debe ubicar el cursor en la parte superior derecha haciendo clic en la opción "Hazte una Cuenta" 
+3. El usuario deja el campo vacio de Email "Indica tu dirección de E-mail"
+4. El usuario debe hacer clic en el botón denominado "Continuar con E-mail"
+5. El usuario evidenciara el siguiente aviso Introduce tu dirección de e-mail"</t>
+  </si>
+  <si>
+    <t>registration failure, empty password fields</t>
+  </si>
+  <si>
+    <t>El usuario no se podrá registrar en la  plataforma Booking por campos vacios en introducir y confirmar la contraseña</t>
+  </si>
+  <si>
+    <t>Ususario:  jagarcia8578@soy.sena.edu.co
+Contraseña: "Campo vacio"
+Confirme contraseña: "Campo vacio"</t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina web https://www.booking.com/ 
+2. El usuario debe ubicar el cursor en la parte superior derecha haciendo clic en la opción "Hazte una Cuenta" 
+3. El usuario ingresara el correo electrónico en el campo "Indica tu dirección de E-mail"
+4. El usuario debe hacer clic en el botón denominado "Continuar con E-mail"
+5. El usuario dejara los dos campos vacios en donde debe ingresar y confirmar la contraseña.
+6. El ususario hara clic en el boto "crear una cuenta" 
+7.El usuario evidenciara los siguientes avisos "Introduce tu dirección de e-mail" y "Confirma tu contraseña"</t>
+  </si>
+  <si>
+    <t>Failed to register, empty fields in enter password</t>
+  </si>
+  <si>
+    <t>El usuario no se podrá registrar en la  plataforma Booking por campo vacio en "introduce contraseña"</t>
+  </si>
+  <si>
+    <t>Ususario:  jagarcia8578@soy.sena.edu.co
+Contraseña: "Campo vacio"
+Confirme contraseña: Prueba123456</t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina web https://www.booking.com/ 
+2. El usuario debe ubicar el cursor en la parte superior derecha haciendo clic en la opción "Hazte una Cuenta" 
+3. El usuario ingresara el correo electrónico en el campo "Indica tu dirección de E-mail"
+4. El usuario debe hacer clic en el botón denominado "Continuar con E-mail"
+5. El usuario dejara el primer campo vacio que dice "Introduce contraseña"
+6. El usuario Ingresa la contraseña en el campo "Confirma la contraseña" 
+7. El ususario hara clic en el boto "Crear una cuenta" 
+8.El usuario evidenciara el siguiente aviso "Las contraseñas no coinciden. Inténtalo de nuevo."</t>
+  </si>
+  <si>
+    <t>failed to register, empty fields in confirm password</t>
+  </si>
+  <si>
+    <t>El usuario no se podrá registrar en la  plataforma Booking por campo vacio en "confirma contraseña"</t>
+  </si>
+  <si>
+    <t>Ususario:  jagarcia8578@soy.sena.edu.co
+Contraseña: Prueba123456
+Confirme contraseña: "Campo vacio"</t>
+  </si>
+  <si>
+    <t>Login Successful</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario se podrá loguear en la  plataforma Booking </t>
   </si>
   <si>
     <t>Usuario: andres.estudio.123@gmail.com
 Contraseña: Prueba123456</t>
-  </si>
-  <si>
-    <t>Ingreso exitoso</t>
-  </si>
-  <si>
-    <t>SI</t>
-  </si>
-  <si>
-    <t>Ingreso fallido</t>
-  </si>
-  <si>
-    <t>Login Fail Password</t>
-  </si>
-  <si>
-    <t>Login Fail Email</t>
-  </si>
-  <si>
-    <t>Usuario: andres.estudio.123@gmail.com
-Contraseña: 123456</t>
   </si>
   <si>
     <t xml:space="preserve">1. El usuario ingresara a la pagina web https://www.booking.com/ 
@@ -120,6 +223,19 @@
   </t>
   </si>
   <si>
+    <t>Ingreso exitoso</t>
+  </si>
+  <si>
+    <t>Login Fail Email</t>
+  </si>
+  <si>
+    <t>El usuario no se podrá loguear en la  plataforma Booking por que el campo de correo no es valido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usuario: andres.estudio.123@gmail
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">1. El usuario ingresara a la pagina web https://www.booking.com/ 
 2. El usuario debe ubicar el curso en la parte superior derecha haciendo clic en la opción "Iniciar sesión" 
 3. El usuario ingresara el correo electrónico erróneo en el campo "Indica tu dirección de E-mail"
@@ -128,89 +244,17 @@
   </t>
   </si>
   <si>
-    <t xml:space="preserve">Usuario: andres.estudio.123@gmail
-</t>
-  </si>
-  <si>
-    <t>El usuario no se podrá loguear en la  plataforma Booking por que el campo de correo no es valido</t>
-  </si>
-  <si>
-    <t>Login Successful</t>
-  </si>
-  <si>
-    <t xml:space="preserve">▪Número de habitaciones: 2.
-▪Número de adultos: 3.
-▪Número de niños: 2.
-</t>
-  </si>
-  <si>
-    <t>Jonathan García y Juan Cajiao</t>
-  </si>
-  <si>
-    <t>campos de reserva funcionales</t>
-  </si>
-  <si>
-    <t>▪Número de habitaciones: 2.
-▪Número de adultos: 3.
-▪Número de niños: 2▪Rango de precio: superior a $200 USD.
-▪Número de estrellas: 3 o más.
-▪Seleccionar el hotel más económico</t>
-  </si>
-  <si>
-    <t>Register Successful</t>
-  </si>
-  <si>
-    <t>Register Fail</t>
-  </si>
-  <si>
-    <t>Login Empty email Field</t>
-  </si>
-  <si>
-    <t>Login Empty Password Field</t>
-  </si>
-  <si>
-    <t>Successful Booking Search</t>
-  </si>
-  <si>
-    <t>Faild Booking Search</t>
-  </si>
-  <si>
-    <t>Failed Reservation Search by Dates</t>
-  </si>
-  <si>
-    <t>Registro exitoso</t>
-  </si>
-  <si>
-    <t>Usuario: jagarcia8578@soy.sena.edu.co
-Contraseña: Prueba123456</t>
-  </si>
-  <si>
-    <t>Usuario: jagarcia8578@soy</t>
-  </si>
-  <si>
-    <t>Registro fallido</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El usuario se podrá registrar en la  plataforma Booking </t>
-  </si>
-  <si>
-    <t>1. El usuario ingresara a la pagina web https://www.booking.com/ 
-2. El usuario debe ubicar el cursor en la parte superior derecha haciendo clic en la opción "Hazte una Cuenta" 
-3. El usuario ingresara el correo electrónico en el campo "Indica tu dirección de E-mail"
-4. El usuario debe hacer clic en el botón denominado "Continuar con E-mail"
-5. El usuario debe ingresar la contraseña en el campo "Introduce tu contraseña"
-6. El usuario debe confirmar la contraseña en el campo "Confirma tu contraseña"
-7.  El usuario debe hacer clic en el botón denominado "Crear una cuentan"
-8. El usuario podrá visualizar la interfaz donde le permite configurar la cuenta.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El usuario no se podrá registrar en la  plataforma Booking </t>
-  </si>
-  <si>
-    <t xml:space="preserve">El usuario se podrá loguear en la  plataforma Booking </t>
+    <t>Ingreso fallido</t>
+  </si>
+  <si>
+    <t>Login Fail Password</t>
   </si>
   <si>
     <t>El usuario no se  podrá loguear en la  plataforma Booking por que el campo de contraseña no es valido</t>
+  </si>
+  <si>
+    <t>Usuario: andres.estudio.123@gmail.com
+Contraseña: 123456</t>
   </si>
   <si>
     <t xml:space="preserve">1. El usuario ingresara a la pagina web https://www.booking.com/ 
@@ -224,6 +268,9 @@
   </t>
   </si>
   <si>
+    <t>Login Empty email Field</t>
+  </si>
+  <si>
     <t>El usuario no se podrá loguear la  plataforma Booking por que el campo de correo esta vacío</t>
   </si>
   <si>
@@ -236,6 +283,9 @@
 4. El usuario debe hacer clic en el botón denominado "Continuar con E-mail"
 5. El usuario no podrá continuar con el logue y evidenciara el mensaje "Introduce tu dirección de e-mail"
   </t>
+  </si>
+  <si>
+    <t>Login Empty Password Field</t>
   </si>
   <si>
     <t>El usuario no se podrá loguear en la  plataforma Booking por que el campo de contraseña esta vacío</t>
@@ -255,7 +305,16 @@
   </t>
   </si>
   <si>
+    <t>Successful Booking Search</t>
+  </si>
+  <si>
     <t xml:space="preserve">El usuario podrá realizar búsquedas de alojamiento en la  plataforma Booking con éxito </t>
+  </si>
+  <si>
+    <t xml:space="preserve">▪Número de habitaciones: 2.
+▪Número de adultos: 3.
+▪Número de niños: 2.
+</t>
   </si>
   <si>
     <t xml:space="preserve">1. El usuario ingresara a la pagina web https://www.booking.com/ 
@@ -275,6 +334,9 @@
     <t xml:space="preserve">Búsqueda exitosa </t>
   </si>
   <si>
+    <t>Faild Booking Search</t>
+  </si>
+  <si>
     <t>El usuario no podrá realizar búsquedas de alojamiento en la  plataforma Booking con éxito</t>
   </si>
   <si>
@@ -295,6 +357,9 @@
     <t xml:space="preserve">Búsqueda fallida </t>
   </si>
   <si>
+    <t>Failed Reservation Search by Dates</t>
+  </si>
+  <si>
     <t>El usuario no podrá realizar búsquedas de alojamiento en la  plataforma Booking con éxito por los campos escogidos en las fechas</t>
   </si>
   <si>
@@ -315,8 +380,22 @@
     <t>El usuario podrá realizar la búsqueda y filtra con el objetivo de completar la reserva</t>
   </si>
   <si>
+    <t>▪Número de habitaciones: 2.
+▪Número de adultos: 3.
+▪Número de niños: 2▪Rango de precio: superior a $200 USD.
+▪Número de estrellas: 3 o más.
+▪Seleccionar el hotel más económico</t>
+  </si>
+  <si>
+    <t>campos de reserva funcionales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">completar la reserva hasta llegar a la interfaz donde solicita la confirmación de la compra   </t>
+  </si>
+  <si>
     <t>1. El usuario ingresara a la pagina web https://www.booking.com/ 
 2. El usuario debe iniciar sesión con anterioridad.
+3. 
 3. El usuario no escogerá el lugar de  destino. 
 4. El usuario escoge la cantidad de días que estará alojado.
 5. El usuario hará clic en apartado  que permite escoger cantidad de adultos, niños y habitaciones que tomaran la reserva.
@@ -337,82 +416,548 @@
 19.  El usuario lograra visualizar el método de pago.</t>
   </si>
   <si>
-    <t xml:space="preserve">completar la reserva hasta llegar a la interfaz donde solicita la confirmación de la compra   </t>
-  </si>
-  <si>
-    <t>ususario: "Campos vacios"</t>
+    <t xml:space="preserve">
+Failed registration due to numerical data</t>
+  </si>
+  <si>
+    <t>El usuario se podrá registrar en la  plataforma Booking por que ingresa unicamente datos numericos en el campo de email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usuario: 123456789
+</t>
+  </si>
+  <si>
+    <t>registration failed due to special characters</t>
+  </si>
+  <si>
+    <t>Usuario:® Ø ă Ὠ ∞ √</t>
+  </si>
+  <si>
+    <t>El usuario se podrá registrar en la  plataforma Booking por que ingresa unicamente caracteres especiales en el campo de email</t>
+  </si>
+  <si>
+    <t>failed login due to insertion of numerical data</t>
+  </si>
+  <si>
+    <t>El usuario no se podrá loguear en la  plataforma Booking por que ingresa datos numericos en el campo de email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usuario:123456789
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. El usuario ingresara a la pagina web https://www.booking.com/ 
+2. El usuario debe ubicar el curso en la parte superior derecha haciendo clic en la opción "Iniciar sesión" 
+3. El usuario ingresara numeros en  el campo "Indica tu dirección de E-mail"
+4. El usuario no podrá ingresar a la plataforma por el correo electrónico erróneo. 
+5. La plataforma mostrará el aviso de "Comprueba si el e-mail que has introducido es correcto"
+  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. El usuario ingresara a la pagina web https://www.booking.com/ 
+2. El usuario debe ubicar el curso en la parte superior derecha haciendo clic en la opción "Iniciar sesión" 
+3. El usuario ingresara caracteres especiales en el campo "Indica tu dirección de E-mail"
+4. El usuario no podrá ingresar a la plataforma por el correo electrónico erróneo. 
+5. La plataforma mostrará el aviso de "Comprueba si el e-mail que has introducido es correcto"
+  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usuario:® Ø ă Ὠ ∞ √
+</t>
+  </si>
+  <si>
+    <t>El usuario no se podrá loguear en la  plataforma Booking por que ingresa caracteres especiales en el campo de email</t>
+  </si>
+  <si>
+    <t>Login failed due to insertion of special characters</t>
   </si>
   <si>
     <t>1. El usuario ingresara a la pagina web https://www.booking.com/ 
 2. El usuario debe ubicar el cursor en la parte superior derecha haciendo clic en la opción "Hazte una Cuenta" 
-3. El usuario ingresara el correo electrónico en el campo "Indica tu dirección de E-mail"
+3. El usuario ingresara numeros en el campo "Indica tu dirección de E-mail"
 4. El usuario debe hacer clic en el botón denominado "Continuar con E-mail"
-5. El usuario evidenciara el siguiente aviso "Comprueba si el e-mail que has introducido es correcto"</t>
-  </si>
-  <si>
-    <t>Failed registration empty fields in email</t>
+5. El usuario evidenciara el siguiente aviso "Comprueba si el e-mail que has introducido es correcto".</t>
   </si>
   <si>
     <t>1. El usuario ingresara a la pagina web https://www.booking.com/ 
 2. El usuario debe ubicar el cursor en la parte superior derecha haciendo clic en la opción "Hazte una Cuenta" 
-3. El usuario deja el campo vacio de Email "Indica tu dirección de E-mail"
+3. El usuario ingresara caracteres especiales en el campo "Indica tu dirección de E-mail"
 4. El usuario debe hacer clic en el botón denominado "Continuar con E-mail"
-5. El usuario evidenciara el siguiente aviso Introduce tu dirección de e-mail"</t>
-  </si>
-  <si>
-    <t>El usuario no se podrá registrar en la  plataforma Booking por campo vacio Email</t>
-  </si>
-  <si>
-    <t>Failed to register, empty fields in enter password</t>
-  </si>
-  <si>
-    <t>failed to register, empty fields in confirm password</t>
-  </si>
-  <si>
-    <t>Ususario:  jagarcia8578@soy.sena.edu.co
-Contraseña: "Campo vacio"
-Confirme contraseña: Prueba123456</t>
-  </si>
-  <si>
-    <t>Ususario:  jagarcia8578@soy.sena.edu.co
-Contraseña: Prueba123456
-Confirme contraseña: "Campo vacio"</t>
-  </si>
-  <si>
-    <t>registration failure, empty password fields</t>
-  </si>
-  <si>
-    <t>Ususario:  jagarcia8578@soy.sena.edu.co
-Contraseña: "Campo vacio"
-Confirme contraseña: "Campo vacio"</t>
+5. El usuario evidenciara el siguiente aviso "Comprueba si el e-mail que has introducido es correcto".</t>
+  </si>
+  <si>
+    <t>Validation of the navigation to the "Vuelos" page.</t>
+  </si>
+  <si>
+    <t>Validation of the navigation to the page "Alquiler de coches".</t>
+  </si>
+  <si>
+    <t>Validation of the navigation to the page "Atracciones turisticas".</t>
+  </si>
+  <si>
+    <t>Validation of the navigation to the page "Taxis Aeropuertos"</t>
+  </si>
+  <si>
+    <t>Validation of the navigation to the page "Alojamiento"</t>
+  </si>
+  <si>
+    <t>El usuario navegara a la pagina Alojamiento para validar que esta siendo redirigido al sitio correspondido</t>
+  </si>
+  <si>
+    <t>El usuario navegara a la pagina Taxis Aeropuertos para validar que esta siendo redirigido al sitio correspondido</t>
+  </si>
+  <si>
+    <t>El usuario navegara a la pagina  Atracciones Turisticas  para validar que esta siendo redirigido al sitio correspondido</t>
+  </si>
+  <si>
+    <t>El usuario navegara a la pagina Alquiler de Coches para validar que esta siendo redirigido al sitio correspondido</t>
+  </si>
+  <si>
+    <t>El usuario navegara a la pagina Vuelos para validar que esta siendo redirigido al sitio correspondido</t>
   </si>
   <si>
     <t>1. El usuario ingresara a la pagina web https://www.booking.com/ 
-2. El usuario debe ubicar el cursor en la parte superior derecha haciendo clic en la opción "Hazte una Cuenta" 
-3. El usuario ingresara el correo electrónico en el campo "Indica tu dirección de E-mail"
-4. El usuario debe hacer clic en el botón denominado "Continuar con E-mail"
-5. El usuario dejara los dos campos vacios en donde debe ingresar y confirmar la contraseña.
-6. El ususario hara clic en el boto "crear una cuenta" 
-7.El usuario evidenciara los siguientes avisos "Introduce tu dirección de e-mail" y "Confirma tu contraseña"</t>
+2. El usuario da clic en "Vuelos"
+3. El usuario visualizara el titulo de "Compara y reserva vuelos fácilmente"</t>
   </si>
   <si>
     <t>1. El usuario ingresara a la pagina web https://www.booking.com/ 
-2. El usuario debe ubicar el cursor en la parte superior derecha haciendo clic en la opción "Hazte una Cuenta" 
-3. El usuario ingresara el correo electrónico en el campo "Indica tu dirección de E-mail"
-4. El usuario debe hacer clic en el botón denominado "Continuar con E-mail"
-5. El usuario dejara el primer campo vacio que dice "Introduce contraseña"
-6. El usuario Ingresa la contraseña en el campo "Confirma la contraseña" 
-7. El ususario hara clic en el boto "Crear una cuenta" 
-8.El usuario evidenciara el siguiente aviso "Las contraseñas no coinciden. Inténtalo de nuevo."</t>
-  </si>
-  <si>
-    <t>El usuario no se podrá registrar en la  plataforma Booking por campos vacios en introducir y confirmar la contraseña</t>
-  </si>
-  <si>
-    <t>El usuario no se podrá registrar en la  plataforma Booking por campo vacio en "introduce contraseña"</t>
-  </si>
-  <si>
-    <t>El usuario no se podrá registrar en la  plataforma Booking por campo vacio en "confirma contraseña"</t>
+2. El usuario da clic en "Alquiler de coches"
+3. El usuario visualizara el titulo de "Alquiler de coches para cualquier tipo de viaje"</t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina web https://www.booking.com/ 
+2. El usuario da clic en "Taxis Aeropuertos"
+3. El usuario visualizara el titulo de "Reserva un taxi desde o al aeropuerto"</t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina web https://www.booking.com/ 
+2. El usuario da clic en "Alojamiento"
+3. El usuario visualizara el titulo de "Encuentra tu próxima estancia"</t>
+  </si>
+  <si>
+    <t>El usuario podra realizar el cambio de idioma de la pagina Booking a Ingles UK</t>
+  </si>
+  <si>
+    <t>Cambio de idioma a Ingles UK</t>
+  </si>
+  <si>
+    <t>Pagina correcta "Vuelos"</t>
+  </si>
+  <si>
+    <t>Pagina correcta "Alquiler de coches"</t>
+  </si>
+  <si>
+    <t>El usuario podra realizar el cambio de idioma de la pagina Booking a Ingles US</t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina web https://www.booking.com/ 
+2. El usuario da clic en la opcion de cambiar idioma
+3. El usuario selecionara el idioma ingles US
+4. El usuario visualizara el idioma de toda la pagna en ingles US</t>
+  </si>
+  <si>
+    <t>Cambio de idioma a Ingles US</t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina web https://www.booking.com/ 
+2. El usuario da clic en la opcion de cambiar idioma
+3. El usuario selecionara el idioma ingles UK
+4. El usuario visualizara el idioma de toda la pagna en ingles UK</t>
+  </si>
+  <si>
+    <t>Validation of language change to "English US"</t>
+  </si>
+  <si>
+    <t>Validation of language change to "English UK"</t>
+  </si>
+  <si>
+    <t>Validation of language change to "French"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario podra realizar el cambio de idioma de la pagina Booking a Frances </t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina web https://www.booking.com/ 
+2. El usuario da clic en "Atracciones Turisticas"
+3. El usuario visualizara el titulo de "Atracciones, actividades y experiencias"</t>
+  </si>
+  <si>
+    <t>Pagina correcta "Atracciones Turisticas"</t>
+  </si>
+  <si>
+    <t>Pagina correcta "Taxis Aeropuertos"</t>
+  </si>
+  <si>
+    <t>Pagina correcta "Alojamiento"</t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina web https://www.booking.com/ 
+2. El usuario da clic en la opcion de cambiar idioma
+3. El usuario selecionara el idioma Frances
+4. El usuario visualizara el idioma de toda la pagina en Frances</t>
+  </si>
+  <si>
+    <t>Pagina correcta</t>
+  </si>
+  <si>
+    <t>Cambio de idioma a Frances</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario podra realizar el cambio de idioma de la pagina Booking a German </t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina web https://www.booking.com/ 
+2. El usuario da clic en la opcion de cambiar idioma
+3. El usuario selecionara el idioma Aleman
+4. El usuario visualizara el idioma de toda la pagina en Aleman</t>
+  </si>
+  <si>
+    <t>Cambio de idioma a Aleman</t>
+  </si>
+  <si>
+    <t>Validation of language change to "German"</t>
+  </si>
+  <si>
+    <t>Validation of language change to "Portuguese"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario podra realizar el cambio de idioma de la pagina Booking a portugues </t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina web https://www.booking.com/ 
+2. El usuario da clic en la opcion de cambiar idioma
+3. El usuario selecionara el idioma portugues
+4. El usuario visualizara el idioma de toda la pagina en portugues</t>
+  </si>
+  <si>
+    <t>Cambio de idioma a portugues</t>
+  </si>
+  <si>
+    <t>validation of the page "Inspírate en tu próximo viaje"</t>
+  </si>
+  <si>
+    <t>Validation of language change to "Italian"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario podra realizar el cambio de idioma de la pagina Booking a Italiano </t>
+  </si>
+  <si>
+    <t>Cambio de idioma a Italiano</t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina web https://www.booking.com/ 
+2. El usuario da clic en la opcion de cambiar idioma
+3. El usuario selecionara el idioma Italiano
+4. El usuario visualizara el idioma de toda la pagina en Italiano</t>
+  </si>
+  <si>
+    <t>El usuario navegara a la pagina  "Articulos" para validar que esta siendo redirigido al sitio correspondido</t>
+  </si>
+  <si>
+    <t>Pagina correcta "Articulos"</t>
+  </si>
+  <si>
+    <t>Validation of language change to "Japanese"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario podra realizar el cambio de idioma de la pagina Booking a Japones </t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina web https://www.booking.com/ 
+2. El usuario da clic en la opcion de cambiar idioma
+3. El usuario selecionara el idioma Japones
+4. El usuario visualizara el idioma de toda la pagina en Japones</t>
+  </si>
+  <si>
+    <t>Cambio de idioma a Japones</t>
+  </si>
+  <si>
+    <t>Validation of language change to "Mandarin"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario podra realizar el cambio de idioma de la pagina Booking a Mandarin </t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina web https://www.booking.com/ 
+2. El usuario da clic en la opcion de cambiar idioma
+3. El usuario selecionara el idioma Mandarin
+4. El usuario visualizara el idioma de toda la pagina en Mandarin</t>
+  </si>
+  <si>
+    <t>Cambio de idioma a Mandarin</t>
+  </si>
+  <si>
+    <t>Validation of the operation of the "Articles" search engine</t>
+  </si>
+  <si>
+    <t>El usuario usara la barra de navegación de "Articulos" para realizar una busqueda</t>
+  </si>
+  <si>
+    <t>*Japon</t>
+  </si>
+  <si>
+    <t>Validation of language change to "Russian "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario podra realizar el cambio de idioma de la pagina Booking a Ruso </t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina web https://www.booking.com/ 
+2. El usuario da clic en la opcion de cambiar idioma
+3. El usuario selecionara el idioma Ruso
+4. El usuario visualizara el idioma de toda la pagina en Ruso</t>
+  </si>
+  <si>
+    <t>Cambio de idioma a Ruso</t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina web https://www.booking.com/articles.html
+2. El usuario da clic en "Articulos"
+3. El usuario visualizara el titulo de "Artículos de viajes"</t>
+  </si>
+  <si>
+    <t>Validation of language change to "Greek  "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario podra realizar el cambio de idioma de la pagina Booking a greco </t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina web https://www.booking.com/ 
+2. El usuario da clic en la opcion de cambiar idioma
+3. El usuario selecionara el idioma greco
+4. El usuario visualizara el idioma de toda la pagina en greco</t>
+  </si>
+  <si>
+    <t>Cambio de idioma a greco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario podra realizar el cambio de idioma de la pagina Booking a Polaco </t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina web https://www.booking.com/ 
+2. El usuario da clic en la opcion de cambiar idioma
+3. El usuario selecionara el idioma Polaco
+4. El usuario visualizara el idioma de toda la pagina en Polaco</t>
+  </si>
+  <si>
+    <t>Cambio de idioma a Polaco</t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina web https://www.booking.com/articles.html
+2. El usuario realiza una busqueda en la barra de navegación de Articulos, donde la palabra a ingresar es Japon
+3. El usuario visualizara articulos que tienen la palabra clave "Japon"</t>
+  </si>
+  <si>
+    <t>Cambio de idioma a Greco</t>
+  </si>
+  <si>
+    <t>Busqueda exitosa de articulos realacionados a Japon</t>
+  </si>
+  <si>
+    <t>Validation of language change to "Portuguese PT"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario podra realizar el cambio de idioma de la pagina Booking a Portuguese PT </t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina web https://www.booking.com/ 
+2. El usuario da clic en la opcion de cambiar idioma
+3. El usuario selecionara el idioma Portuguese PT
+4. El usuario visualizara el idioma de toda la pagina en Portuguese PT</t>
+  </si>
+  <si>
+    <t>Cambio de idioma a Portuguese PT</t>
+  </si>
+  <si>
+    <t>Validation of the operation of the "Articles" search engine without words</t>
+  </si>
+  <si>
+    <t>El usuario usara la barra de navegación de "Articulos" para realizar una busqueda sin ninguna palabra clave</t>
+  </si>
+  <si>
+    <t>Validation of language change to "Filipino   "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario podra realizar el cambio de idioma de la pagina Booking a Filipino  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. El usuario ingresara a la pagina web https://www.booking.com/ 
+2. El usuario da clic en la opcion de cambiar idioma
+3. El usuario selecionara el idioma Filipino 
+4. El usuario visualizara el idioma de toda la pagina en Filipino </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cambio de idioma a Filipino </t>
+  </si>
+  <si>
+    <t>Validation of language change to "Polish"</t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina web https://www.booking.com/articles.html
+2. El usuario realiza una busqueda en la barra de navegación de Articulos, donde no ingresara ninguna dato
+3. El usuario visualizara un mensaje de "No se ha encontrado la página"</t>
+  </si>
+  <si>
+    <t>Redireccionamiento a pagina "No se ha encontrado la pagina"</t>
+  </si>
+  <si>
+    <t>El usuario no ingresa el correo y da clic en enviar en el formulario de "Ahorra tiempo y dinero"</t>
+  </si>
+  <si>
+    <t>successful entry to the extranet</t>
+  </si>
+  <si>
+    <t>El usuario navegara a la pagina  "Extranet" para validar que esta siendo redirigido al sitio correspondido</t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina web https://www.booking.com/
+2. El usuario da clic en "Suscribete"
+3. El usuario visualizara un mensaje de error "Rellene este campo"</t>
+  </si>
+  <si>
+    <t>El usuario visualizara un mensaje de error "Rellene este campo"</t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina web https://www.booking.com
+2.El usuario se desplazara hasta debajo de la pagina.
+3. El usuario da clic en el apartado que dice "Acceso a la extranet"
+4. El usuario visualizara el acceso a la extranet visualizando el titulo de "Inicia sesión para gestionar tu establecimiento"</t>
+  </si>
+  <si>
+    <t>Validation of the "Save time and money" form without entering your email address</t>
+  </si>
+  <si>
+    <t>Validation of the "Save time and money" form with numbers</t>
+  </si>
+  <si>
+    <t>Validation of "Save time and money" form letters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validation of the "Save time and money" form with symbols </t>
+  </si>
+  <si>
+    <t>Pagina Correcta "Intranet"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validation of "Save time and money" form with alphanumeric  </t>
+  </si>
+  <si>
+    <t>El usurio ingresa numeros en el formulario y da clic en enviar el formulario de "Ahorra tiempo y dinero"</t>
+  </si>
+  <si>
+    <t>El usurio ingresa unicament letras en el formulario y da clic en enviar el formulario de "Ahorra tiempo y dinero"</t>
+  </si>
+  <si>
+    <t>El usurio ingresa simbolos en el formulario y da clic en enviar el formulario de "Ahorra tiempo y dinero"</t>
+  </si>
+  <si>
+    <t>El usurio ingresa correo electronico en el formulario y da clic en enviar el formulario de "Ahorra tiempo y dinero"</t>
+  </si>
+  <si>
+    <t>Login failed due to insertion of special characters in the extranet</t>
+  </si>
+  <si>
+    <t>* }{+{{´{}´-?%%"</t>
+  </si>
+  <si>
+    <t>* poloatierrastranger</t>
+  </si>
+  <si>
+    <t>El usuario ingresa a la extranet e ingresa caracteres especiales en el nombre de usuario</t>
+  </si>
+  <si>
+    <t>* 23536453</t>
+  </si>
+  <si>
+    <t>* jaun12323</t>
+  </si>
+  <si>
+    <t>* holamundo@gmail.com</t>
+  </si>
+  <si>
+    <t>Inicio de sesion fallido extranet</t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina web https://www.booking.com/
+2. El usuario ingresa numeros en el formulario "Ahorra tiempo y dinero"
+2. El usuario da clic en "Suscribete"
+3. El usuario visualizara un mensaje de error "Incluye una '@' en la direccion de correo electronico. A '23536453' le falta una '@'"</t>
+  </si>
+  <si>
+    <t>Login failed due to insertion of numbers  in the extranet</t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina web https://www.booking.com/
+2. El usuario ingresa letras en el formulario "Ahorra tiempo y dinero"
+2. El usuario da clic en "Suscribete"
+3. El usuario visualizara un mensaje de error "Incluye una '@' en la direccion de correo electronico. A 'poloatierrastranger' le falta una '@'"</t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina de de intranet 
+2. El usuario ingresara numeros  en el campo "Nombre de usuario"
+3. El usuasrio visualizara el mensaje de "Parece que no existe ninguna cuenta con este nombre de usuario. Crea una cuenta para acceder a nuestros servicios"</t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina de de intranet 
+2. El usuario ingresara caracteres especiales en el campo "Nombre de usuario"
+3. El usuasrio visualizara el mensaje de "Parece que no existe ninguna cuenta con este nombre de usuario. Crea una cuenta para acceder a nuestros servicios"</t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina web https://www.booking.com/
+2. El usuario ingresa simbolos en el formulario "Ahorra tiempo y dinero"
+2. El usuario da clic en "Suscribete"
+3. El usuario visualizara un mensaje de error "Incluye una '@' en la direccion de correo electronico. A '}{+{{´{}´-?%%"' le falta una '@'"</t>
+  </si>
+  <si>
+    <t>Usuario:1232543454</t>
+  </si>
+  <si>
+    <t>Usuario:PruebaSena2023</t>
+  </si>
+  <si>
+    <t>Login failed due to insertion of alphanumeric  in the extranet</t>
+  </si>
+  <si>
+    <t>El usuario ingresa a la extranet e ingresa caracteres alfanumericos en el nombre de usuario</t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina web https://www.booking.com/
+2. El usuario ingresa correo electronico en el formulario "Ahorra tiempo y dinero"
+2. El usuario da clic en "Suscribete"
+3. El usuario visualizara un mensaje de confirmación "¡Gracias! Te hemos enviado un e-mail para que puedas completar la suscripción"</t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina de de intranet 
+2. El usuario ingresara carateres alfanumericos  en el campo "Nombre de usuario"
+3. El usuasrio visualizara el mensaje de "Parece que no existe ninguna cuenta con este nombre de usuario. Crea una cuenta para acceder a nuestros servicios"</t>
+  </si>
+  <si>
+    <t>El usuario visualizara un mensaje de error "Incluye una '@' en la direccion de correo electronico. A '23536453' le falta una '@'"</t>
+  </si>
+  <si>
+    <t>El usuario visualizara un mensaje de error "Incluye una '@' en la direccion de correo electronico. A 'poloatierrastranger' le falta una '@'"</t>
+  </si>
+  <si>
+    <t>El usuario visualizara un mensaje de error "Incluye una '@' en la direccion de correo electronico. A '}{+{{´{}´-?%%"' le falta una '@'"</t>
+  </si>
+  <si>
+    <t>El usuario visualizara un mensaje de confirmación "¡Gracias! Te hemos enviado un e-mail para que puedas completar la suscripción"</t>
+  </si>
+  <si>
+    <t>El usuario ingresa alfanumérico en el formulario y da clic en enviar el formulario de "Ahorra tiempo y dinero"</t>
+  </si>
+  <si>
+    <t>1. El usuario ingresara a la pagina web https://www.booking.com/
+2. El usuario ingresa una palabra alfanumérica en el formulario "Ahorra tiempo y dinero"
+2. El usuario da clic en "Suscríbete"
+3. El usuario visualizara un mensaje de error "Incluye una '@' en la dirección de correo electrónico. A 'jaun12323' le falta una '@'"</t>
+  </si>
+  <si>
+    <t>El usuario visualizara un mensaje de error "Incluye una '@' en la dirección de correo electrónico. A 'jaun12323' le falta una '@'"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validación of the "Save Time and Money" form with mailing  </t>
   </si>
 </sst>
 </file>
@@ -842,21 +1387,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5A7B641-343E-474D-976F-032D518AA969}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" customWidth="1"/>
     <col min="3" max="3" width="48" customWidth="1"/>
     <col min="4" max="4" width="49.7109375" customWidth="1"/>
     <col min="5" max="5" width="68.42578125" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.42578125" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" customWidth="1"/>
     <col min="10" max="10" width="18.85546875" customWidth="1"/>
@@ -865,58 +1410,58 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="230.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -924,464 +1469,1505 @@
         <v>1</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="2"/>
       <c r="J6" s="6" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="230.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>2</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="2"/>
       <c r="J7" s="6" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="230.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>3</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="2"/>
       <c r="J8" s="6" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="189.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>4</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>82</v>
+        <v>24</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>79</v>
+        <v>25</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>80</v>
+        <v>26</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="2"/>
       <c r="J9" s="6" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="203.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>5</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>83</v>
+        <v>29</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>76</v>
+        <v>30</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>81</v>
+        <v>31</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="H10" s="8"/>
       <c r="I10" s="2"/>
       <c r="J10" s="6" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="217.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="189.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>6</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>75</v>
+        <v>32</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>77</v>
+        <v>34</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>81</v>
+        <v>35</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="2"/>
       <c r="J11" s="6" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="218.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="203.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>7</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="G12" s="6" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="2"/>
       <c r="J12" s="6" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="217.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>8</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="H13" s="8"/>
       <c r="I13" s="2"/>
       <c r="J13" s="6" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="210" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="218.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>9</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C14" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="G14" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" s="9"/>
-      <c r="I14" s="1"/>
+        <v>47</v>
+      </c>
+      <c r="H14" s="8"/>
+      <c r="I14" s="2"/>
       <c r="J14" s="6" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="218.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>10</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>50</v>
+        <v>92</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>93</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>51</v>
+        <v>94</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="1"/>
+        <v>52</v>
+      </c>
+      <c r="H15" s="8"/>
+      <c r="I15" s="2"/>
       <c r="J15" s="6" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="218.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>11</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>35</v>
+        <v>98</v>
       </c>
       <c r="C16" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="G16" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="1"/>
+        <v>52</v>
+      </c>
+      <c r="H16" s="8"/>
+      <c r="I16" s="2"/>
       <c r="J16" s="6" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="165" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>12</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H17" s="9"/>
-      <c r="I17" s="1"/>
+        <v>52</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" s="8"/>
+      <c r="I17" s="2"/>
       <c r="J17" s="6" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="188.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="210" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>13</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>62</v>
+        <v>52</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="1"/>
       <c r="J18" s="6" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="195" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>14</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>28</v>
+        <v>58</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>62</v>
+        <v>52</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="1"/>
       <c r="J19" s="6" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="375" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>15</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="H20" s="9"/>
       <c r="I20" s="1"/>
       <c r="J20" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="165" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>16</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H21" s="9"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="188.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>17</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H22" s="9"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="195" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>18</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H23" s="9"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>19</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H24" s="9"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>20</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H25" s="9"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>21</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H26" s="9"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>22</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H27" s="9"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>23</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H28" s="9"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>24</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="H29" s="9"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>25</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="H30" s="9"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>26</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="H31" s="9"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>27</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="H32" s="9"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>28</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="H33" s="9"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
         <v>29</v>
       </c>
-      <c r="K20" s="2" t="s">
-        <v>18</v>
+      <c r="B34" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="H34" s="9"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>30</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="H35" s="9"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>31</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="H36" s="9"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>32</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="H37" s="9"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>33</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="H38" s="9"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>34</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="H39" s="9"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>35</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="H40" s="9"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>36</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="H41" s="9"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="390" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>37</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H42" s="9"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>38</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="H43" s="9"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>39</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="H44" s="9"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>40</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="H45" s="9"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>41</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="H46" s="9"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>42</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="H47" s="9"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>43</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H48" s="9"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>44</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="H49" s="9"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>45</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="H50" s="9"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K50" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>46</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="H51" s="9"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K51" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>47</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="H52" s="9"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>48</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="H53" s="9"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>49</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="H54" s="9"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K54" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>50</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="H55" s="9"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K55" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1401,7 +2987,7 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Juanes Update Login Scenario
</commit_message>
<xml_diff>
--- a/Documentos/PTP_Juan_Cajoia_Jonathan_ Garcia_26092023 .xlsx
+++ b/Documentos/PTP_Juan_Cajoia_Jonathan_ Garcia_26092023 .xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AdminSena\Documents\GitHub\Senasoft2023Grupo15\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{36F89E65-23F6-4CFF-8FAF-8912E2678A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE746DB-9EED-45FA-85E6-BA0D9419A5D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D20512B1-8783-41FD-B729-50DEFE0AFE11}"/>
   </bookViews>
@@ -1084,10 +1084,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1389,8 +1385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5A7B641-343E-474D-976F-032D518AA969}">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2815,7 +2811,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
Update Scenario Form Contact Us
Esta incompleto, debemos investigar validación con javascript
</commit_message>
<xml_diff>
--- a/Documentos/PTP_Juan_Cajoia_Jonathan_ Garcia_26092023 .xlsx
+++ b/Documentos/PTP_Juan_Cajoia_Jonathan_ Garcia_26092023 .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AdminSena\Documents\GitHub\Senasoft2023Grupo15\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAA912E-D5D9-4F5B-9DD6-59B846FE4950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A085FC-9B96-4E3C-8143-E56E66DADA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D20512B1-8783-41FD-B729-50DEFE0AFE11}"/>
   </bookViews>
@@ -1385,13 +1385,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5A7B641-343E-474D-976F-032D518AA969}">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" customWidth="1"/>
     <col min="3" max="3" width="48" customWidth="1"/>
     <col min="4" max="4" width="49.7109375" customWidth="1"/>

</xml_diff>

<commit_message>
Create change language options
</commit_message>
<xml_diff>
--- a/Documentos/PTP_Juan_Cajoia_Jonathan_ Garcia_26092023 .xlsx
+++ b/Documentos/PTP_Juan_Cajoia_Jonathan_ Garcia_26092023 .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AdminSena\Documents\GitHub\Senasoft2023Grupo15\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A085FC-9B96-4E3C-8143-E56E66DADA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F403D82-D889-4059-9F24-F6D40BBC41E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D20512B1-8783-41FD-B729-50DEFE0AFE11}"/>
   </bookViews>
@@ -776,9 +776,6 @@
     <t>El usuario usara la barra de navegación de "Articulos" para realizar una busqueda sin ninguna palabra clave</t>
   </si>
   <si>
-    <t>Validation of language change to "Filipino   "</t>
-  </si>
-  <si>
     <t xml:space="preserve">El usuario podra realizar el cambio de idioma de la pagina Booking a Filipino  </t>
   </si>
   <si>
@@ -958,6 +955,9 @@
   </si>
   <si>
     <t xml:space="preserve">Validación of the "Save Time and Money" form with mailing  </t>
+  </si>
+  <si>
+    <t>Validation of language change to "Filipino"</t>
   </si>
 </sst>
 </file>
@@ -1385,8 +1385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5A7B641-343E-474D-976F-032D518AA969}">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2487,7 +2487,7 @@
         <v>35</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>169</v>
@@ -2516,20 +2516,20 @@
         <v>36</v>
       </c>
       <c r="B41" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="C41" s="6" t="s">
         <v>181</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>182</v>
       </c>
       <c r="D41" s="7"/>
       <c r="E41" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="F41" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="F41" s="6" t="s">
-        <v>184</v>
-      </c>
       <c r="G41" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H41" s="9"/>
       <c r="I41" s="1"/>
@@ -2576,20 +2576,20 @@
         <v>38</v>
       </c>
       <c r="B43" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C43" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="D43" s="7"/>
       <c r="E43" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H43" s="9"/>
       <c r="I43" s="1"/>
@@ -2605,22 +2605,22 @@
         <v>39</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>89</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H44" s="9"/>
       <c r="I44" s="1"/>
@@ -2636,22 +2636,22 @@
         <v>40</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H45" s="9"/>
       <c r="I45" s="1"/>
@@ -2667,22 +2667,22 @@
         <v>41</v>
       </c>
       <c r="B46" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="C46" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="C46" s="6" t="s">
-        <v>221</v>
-      </c>
       <c r="D46" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H46" s="9"/>
       <c r="I46" s="1"/>
@@ -2765,13 +2765,13 @@
       </c>
       <c r="D49" s="7"/>
       <c r="E49" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="F49" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="F49" s="6" t="s">
-        <v>187</v>
-      </c>
       <c r="G49" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H49" s="9"/>
       <c r="I49" s="1"/>
@@ -2787,20 +2787,20 @@
         <v>45</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D50" s="7"/>
       <c r="E50" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="F50" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="F50" s="6" t="s">
-        <v>192</v>
-      </c>
       <c r="G50" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H50" s="9"/>
       <c r="I50" s="1"/>
@@ -2816,22 +2816,22 @@
         <v>46</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H51" s="9"/>
       <c r="I51" s="1"/>
@@ -2847,22 +2847,22 @@
         <v>47</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H52" s="9"/>
       <c r="I52" s="1"/>
@@ -2878,22 +2878,22 @@
         <v>48</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H53" s="9"/>
       <c r="I53" s="1"/>
@@ -2909,22 +2909,22 @@
         <v>49</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C54" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="E54" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="D54" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="E54" s="7" t="s">
+      <c r="F54" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="F54" s="6" t="s">
-        <v>230</v>
-      </c>
       <c r="G54" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H54" s="9"/>
       <c r="I54" s="1"/>
@@ -2940,22 +2940,22 @@
         <v>50</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H55" s="9"/>
       <c r="I55" s="1"/>

</xml_diff>